<commit_message>
feat: Integrar captura de saldos en Banco Estado
- Agregar import de saldo_bancos_db en Scrap_estado.py
- Implementar función capturar_saldo_cuenta() para extraer saldo después del login
- Agregar función normalizar_saldo() con formato chileno (punto como separador de miles)
- Implementar función guardar_saldo_estado() para persistir saldos en BD
- Integrar captura de saldos en process_account() antes del procesamiento de transferencias
- Corregir manejo de formato monetario chileno (sin decimales)
- Agregar scripts auxiliares para diagnóstico y manejo de saldos BCI
</commit_message>
<xml_diff>
--- a/EXCEL_SANTANDER/000091404630.xlsx
+++ b/EXCEL_SANTANDER/000091404630.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <x:si>
     <x:t>Consulta de movimientos de Cuentas Corrientes</x:t>
   </x:si>
@@ -28,7 +28,7 @@
     <x:t>Fecha:</x:t>
   </x:si>
   <x:si>
-    <x:t>24 de julio de 2025</x:t>
+    <x:t>30 de julio de 2025</x:t>
   </x:si>
   <x:si>
     <x:t>Empresa:</x:t>
@@ -40,7 +40,7 @@
     <x:t>Hora:</x:t>
   </x:si>
   <x:si>
-    <x:t>14:28</x:t>
+    <x:t>18:31</x:t>
   </x:si>
   <x:si>
     <x:t>RUT empresa:</x:t>
@@ -169,7 +169,7 @@
         <x:rFont val="Calibri"/>
         <x:family val="2"/>
       </x:rPr>
-      <x:t>17/07/2025</x:t>
+      <x:t>23/07/2025</x:t>
     </x:r>
   </x:si>
   <x:si>
@@ -192,7 +192,7 @@
         <x:rFont val="Calibri"/>
         <x:family val="2"/>
       </x:rPr>
-      <x:t>31/07/2025</x:t>
+      <x:t>06/08/2025</x:t>
     </x:r>
   </x:si>
   <x:si>
@@ -295,6 +295,684 @@
         <x:rFont val="Calibri"/>
         <x:family val="2"/>
       </x:rPr>
+      <x:t>Transf.Internet a 77.920.777-3</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>30/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:t>C</x:t>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>0777734482 Transf. SAN CRISTOBAL SPA</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>30/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:t>A</x:t>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>Transf.Internet a 78.013.487-9</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>30/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>Transf.Internet a 16.833.612-8</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>30/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>077936187K Transf. ST CRISTOBAL SPA</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>30/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>COM.MANTENCION PLAN</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>29/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>0271111576 Transf de KARINA ALEJANDRA AL</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>30/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>OTRAS GERENCIAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>00761072935 Tranf. Internet de 78.107.2935</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>29/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>OPERACIONES CENTRALES</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>0265234356 Transf. ORTA MARTINEZ JESUS ANTONIO</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>28/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>0263855957 Transf a EDUARDO JOSE MONTILLA NORIEG</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>28/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>Transf.Internet a 77.920.777-3</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>25/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>077936187K Transf. ST CRISTOBAL SPA</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>25/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>0271111576 Transf de KARINA ALEJANDRA AL</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>25/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>OTRAS GERENCIAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>0777734482 Transf. SAN CRISTOBAL SPA</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>25/07/2025</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>000000000</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>AGUSTINAS</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="10"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
       <x:t>0772582234 Transf a Aguacate Investments SpA</x:t>
     </x:r>
   </x:si>
@@ -332,492 +1010,6 @@
         <x:family val="2"/>
       </x:rPr>
       <x:t>AGUSTINAS</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:t>C</x:t>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>0265234356 Transf de JESUS ANTONIO ORTA</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>22/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>OTRAS GERENCIAS</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:t>A</x:t>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>PAGO EN LINEA S.I.I.</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>21/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>OTRAS GERENCIAS</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>0777734482 Transf. SAN CRISTOBAL SPA</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>21/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>AGUSTINAS</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>0268574255 Transf a Liliana Gil</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>21/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>AGUSTINAS</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>Transf.Internet a 77.969.191-8</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>21/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>AGUSTINAS</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>0271111576 Transf de KARINA ALEJANDRA AL</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>21/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>OTRAS GERENCIAS</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>PAGO EN LINEA S.I.I.</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>17/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>OTRAS GERENCIAS</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>00761072935 Tranf. Internet de 78.107.2935</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>17/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>OPERACIONES CENTRALES</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>00761072935 Tranf. Internet de 78.107.2935</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>17/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>OPERACIONES CENTRALES</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>0265234356 Transf de JESUS ANTONIO ORTA</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>17/07/2025</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>000000000</x:t>
-    </x:r>
-  </x:si>
-  <x:si>
-    <x:r>
-      <x:rPr>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="10"/>
-        <x:color rgb="FF000000"/>
-        <x:rFont val="Calibri"/>
-        <x:family val="2"/>
-      </x:rPr>
-      <x:t>OTRAS GERENCIAS</x:t>
     </x:r>
   </x:si>
 </x:sst>
@@ -1264,7 +1456,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G23"/>
+  <x:dimension ref="A1:G27"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1489,7 +1681,7 @@
     </x:row>
     <x:row r="13" spans="1:7">
       <x:c r="A13" s="7" t="n">
-        <x:v>-600000</x:v>
+        <x:v>-3400000</x:v>
       </x:c>
       <x:c r="B13" s="3" t="s">
         <x:v>27</x:v>
@@ -1498,7 +1690,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="D13" s="7" t="n">
-        <x:v>17446</x:v>
+        <x:v>63347</x:v>
       </x:c>
       <x:c r="E13" s="3" t="s">
         <x:v>29</x:v>
@@ -1512,7 +1704,7 @@
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="7" t="n">
-        <x:v>200000</x:v>
+        <x:v>800000</x:v>
       </x:c>
       <x:c r="B14" s="3" t="s">
         <x:v>32</x:v>
@@ -1521,7 +1713,7 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="D14" s="7" t="n">
-        <x:v>617446</x:v>
+        <x:v>3463347</x:v>
       </x:c>
       <x:c r="E14" s="3" t="s">
         <x:v>34</x:v>
@@ -1535,7 +1727,7 @@
     </x:row>
     <x:row r="15" spans="1:7">
       <x:c r="A15" s="7" t="n">
-        <x:v>-35000</x:v>
+        <x:v>-3900000</x:v>
       </x:c>
       <x:c r="B15" s="3" t="s">
         <x:v>37</x:v>
@@ -1544,7 +1736,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="D15" s="7" t="n">
-        <x:v>417446</x:v>
+        <x:v>2663347</x:v>
       </x:c>
       <x:c r="E15" s="3" t="s">
         <x:v>39</x:v>
@@ -1558,7 +1750,7 @@
     </x:row>
     <x:row r="16" spans="1:7">
       <x:c r="A16" s="7" t="n">
-        <x:v>361500</x:v>
+        <x:v>-4000000</x:v>
       </x:c>
       <x:c r="B16" s="3" t="s">
         <x:v>41</x:v>
@@ -1567,7 +1759,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="D16" s="7" t="n">
-        <x:v>452446</x:v>
+        <x:v>6563347</x:v>
       </x:c>
       <x:c r="E16" s="3" t="s">
         <x:v>43</x:v>
@@ -1576,12 +1768,12 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="G16" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:7">
       <x:c r="A17" s="7" t="n">
-        <x:v>-75000</x:v>
+        <x:v>7000000</x:v>
       </x:c>
       <x:c r="B17" s="3" t="s">
         <x:v>45</x:v>
@@ -1590,7 +1782,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="D17" s="7" t="n">
-        <x:v>90946</x:v>
+        <x:v>10563347</x:v>
       </x:c>
       <x:c r="E17" s="3" t="s">
         <x:v>47</x:v>
@@ -1599,12 +1791,12 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="G17" s="3" t="s">
-        <x:v>31</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:7">
       <x:c r="A18" s="7" t="n">
-        <x:v>-7000000</x:v>
+        <x:v>-19241</x:v>
       </x:c>
       <x:c r="B18" s="3" t="s">
         <x:v>49</x:v>
@@ -1613,7 +1805,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="D18" s="7" t="n">
-        <x:v>165946</x:v>
+        <x:v>3563347</x:v>
       </x:c>
       <x:c r="E18" s="3" t="s">
         <x:v>51</x:v>
@@ -1627,7 +1819,7 @@
     </x:row>
     <x:row r="19" spans="1:7">
       <x:c r="A19" s="7" t="n">
-        <x:v>70000</x:v>
+        <x:v>30000</x:v>
       </x:c>
       <x:c r="B19" s="3" t="s">
         <x:v>53</x:v>
@@ -1636,7 +1828,7 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="D19" s="7" t="n">
-        <x:v>7165946</x:v>
+        <x:v>3582588</x:v>
       </x:c>
       <x:c r="E19" s="3" t="s">
         <x:v>55</x:v>
@@ -1650,7 +1842,7 @@
     </x:row>
     <x:row r="20" spans="1:7">
       <x:c r="A20" s="7" t="n">
-        <x:v>-628948</x:v>
+        <x:v>48850</x:v>
       </x:c>
       <x:c r="B20" s="3" t="s">
         <x:v>57</x:v>
@@ -1659,7 +1851,7 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="D20" s="7" t="n">
-        <x:v>7095946</x:v>
+        <x:v>3552588</x:v>
       </x:c>
       <x:c r="E20" s="3" t="s">
         <x:v>59</x:v>
@@ -1668,12 +1860,12 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="G20" s="3" t="s">
-        <x:v>31</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:7">
       <x:c r="A21" s="7" t="n">
-        <x:v>6592173</x:v>
+        <x:v>4000</x:v>
       </x:c>
       <x:c r="B21" s="3" t="s">
         <x:v>61</x:v>
@@ -1682,7 +1874,7 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="D21" s="7" t="n">
-        <x:v>7724894</x:v>
+        <x:v>3503738</x:v>
       </x:c>
       <x:c r="E21" s="3" t="s">
         <x:v>63</x:v>
@@ -1696,7 +1888,7 @@
     </x:row>
     <x:row r="22" spans="1:7">
       <x:c r="A22" s="7" t="n">
-        <x:v>641550</x:v>
+        <x:v>-7708</x:v>
       </x:c>
       <x:c r="B22" s="3" t="s">
         <x:v>65</x:v>
@@ -1705,7 +1897,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="D22" s="7" t="n">
-        <x:v>1132721</x:v>
+        <x:v>3499738</x:v>
       </x:c>
       <x:c r="E22" s="3" t="s">
         <x:v>67</x:v>
@@ -1714,12 +1906,12 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="G22" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:7">
       <x:c r="A23" s="7" t="n">
-        <x:v>16138</x:v>
+        <x:v>-4000000</x:v>
       </x:c>
       <x:c r="B23" s="3" t="s">
         <x:v>69</x:v>
@@ -1728,7 +1920,7 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="D23" s="7" t="n">
-        <x:v>491171</x:v>
+        <x:v>3507446</x:v>
       </x:c>
       <x:c r="E23" s="3" t="s">
         <x:v>71</x:v>
@@ -1737,7 +1929,99 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="G23" s="3" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:7">
+      <x:c r="A24" s="7" t="n">
+        <x:v>7000000</x:v>
+      </x:c>
+      <x:c r="B24" s="3" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C24" s="3" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D24" s="7" t="n">
+        <x:v>7507446</x:v>
+      </x:c>
+      <x:c r="E24" s="3" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="F24" s="3" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G24" s="3" t="s">
         <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:7">
+      <x:c r="A25" s="7" t="n">
+        <x:v>40000</x:v>
+      </x:c>
+      <x:c r="B25" s="3" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C25" s="3" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="D25" s="7" t="n">
+        <x:v>507446</x:v>
+      </x:c>
+      <x:c r="E25" s="3" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F25" s="3" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="G25" s="3" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:7">
+      <x:c r="A26" s="7" t="n">
+        <x:v>450000</x:v>
+      </x:c>
+      <x:c r="B26" s="3" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C26" s="3" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="D26" s="7" t="n">
+        <x:v>467446</x:v>
+      </x:c>
+      <x:c r="E26" s="3" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="F26" s="3" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="G26" s="3" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:7">
+      <x:c r="A27" s="7" t="n">
+        <x:v>-600000</x:v>
+      </x:c>
+      <x:c r="B27" s="3" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="C27" s="3" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="D27" s="7" t="n">
+        <x:v>17446</x:v>
+      </x:c>
+      <x:c r="E27" s="3" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="F27" s="3" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="G27" s="3" t="s">
+        <x:v>31</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>